<commit_message>
update notebook, data, image
</commit_message>
<xml_diff>
--- a/data/korea_map_21th_election_type_b.xlsx
+++ b/data/korea_map_21th_election_type_b.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baem1n/PROJECT/PycharmProjects/korea-election-analysis /data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\korea-election-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16971567-8FA7-D248-AD1A-089A6559202F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="1280" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8700" yWindow="1280" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -787,8 +786,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1152,19 +1151,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="17" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="50" customHeight="1">
+    <row r="1" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1217,7 +1216,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="50" customHeight="1">
+    <row r="2" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1240,7 +1239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="50" customHeight="1">
+    <row r="3" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="50" customHeight="1">
+    <row r="4" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1310,7 +1309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="50" customHeight="1">
+    <row r="5" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="50" customHeight="1">
+    <row r="6" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="50" customHeight="1">
+    <row r="7" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1427,7 +1426,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="50" customHeight="1">
+    <row r="8" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1468,7 +1467,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="50" customHeight="1">
+    <row r="9" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1515,7 +1514,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="50" customHeight="1">
+    <row r="10" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1562,7 +1561,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="50" customHeight="1">
+    <row r="11" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1612,7 +1611,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="50" customHeight="1">
+    <row r="12" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="50" customHeight="1">
+    <row r="13" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1709,7 +1708,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="50" customHeight="1">
+    <row r="14" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="50" customHeight="1">
+    <row r="15" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1800,7 +1799,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="50" customHeight="1">
+    <row r="16" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="50" customHeight="1">
+    <row r="17" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1882,7 +1881,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="50" customHeight="1">
+    <row r="18" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="50" customHeight="1">
+    <row r="19" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1970,7 +1969,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="50" customHeight="1">
+    <row r="20" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="50" customHeight="1">
+    <row r="21" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="50" customHeight="1">
+    <row r="22" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2072,7 +2071,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="50" customHeight="1">
+    <row r="23" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>

</xml_diff>